<commit_message>
changed the docker-compose.yml file to add the docker host, to access ollama service. created a tutorial to setup PGVector on the postgres docker container instance
</commit_message>
<xml_diff>
--- a/data/mylibrary/mylibrary.xlsx
+++ b/data/mylibrary/mylibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fb35ef21df554d5/Documents/Books to Read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80050CA0-8D3E-48BA-BD84-E8E96811E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{80050CA0-8D3E-48BA-BD84-E8E96811E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{785AFE10-494F-4E10-906B-39FFCA1E429C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB081F56-E215-4A57-8E05-68661072F278}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
-  <si>
-    <t>Titile</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>ISBN</t>
   </si>
@@ -104,9 +101,6 @@
     <t>Modern Data Architecture on AWS</t>
   </si>
   <si>
-    <t>Packt Publishingg</t>
-  </si>
-  <si>
     <t>Behram Irani</t>
   </si>
   <si>
@@ -168,6 +162,72 @@
   </si>
   <si>
     <t>MLOps, machine learning</t>
+  </si>
+  <si>
+    <t>Generative AI on AWS</t>
+  </si>
+  <si>
+    <t>Chris Fregly, Antje Barth,Shelbee Eigenbrode</t>
+  </si>
+  <si>
+    <t>978-1-098-15922-1</t>
+  </si>
+  <si>
+    <t>aws,generative ai, large language models,deep learning</t>
+  </si>
+  <si>
+    <t>Pattern Recognition and Machine Learning</t>
+  </si>
+  <si>
+    <t>Springer</t>
+  </si>
+  <si>
+    <t>Christopher M. Bishop</t>
+  </si>
+  <si>
+    <t>machine learning, ml algorithms, deep learning</t>
+  </si>
+  <si>
+    <t>978-0387-31073-2</t>
+  </si>
+  <si>
+    <t>Christopher M. Bishop, Hugh Bishop</t>
+  </si>
+  <si>
+    <t>Deep Learning Foundations and Concepts</t>
+  </si>
+  <si>
+    <t>978-3-031-45467-7</t>
+  </si>
+  <si>
+    <t>15 Math Concepts Every Data Scientist Should Know</t>
+  </si>
+  <si>
+    <t>David Hoyle</t>
+  </si>
+  <si>
+    <t>mathematics, machine learning, deep learning, data science</t>
+  </si>
+  <si>
+    <t>Packt Publishing</t>
+  </si>
+  <si>
+    <t>978-1-83763-418-7</t>
+  </si>
+  <si>
+    <t>DevSecOps for Azure</t>
+  </si>
+  <si>
+    <t>978-1-83763-111-7</t>
+  </si>
+  <si>
+    <t>David Okeyode, Joylynn Kirui</t>
+  </si>
+  <si>
+    <t>devsecops, azure, cloud</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -540,9 +600,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493EB18A-A9C7-4C4D-B1C1-94DC4EF06034}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -556,68 +618,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>2024</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,91 +687,91 @@
         <v>9780593185742</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>2024</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>2023</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>2024</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>2023</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,22 +779,22 @@
         <v>9781617296529</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>2020</v>
       </c>
       <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
         <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,22 +802,137 @@
         <v>9781617297762</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>2022</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="G9" t="s">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>2024</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2006</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>2024</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>2024</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>2024</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed basic tutorials for elasticserch
</commit_message>
<xml_diff>
--- a/data/mylibrary/mylibrary.xlsx
+++ b/data/mylibrary/mylibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fb35ef21df554d5/Documents/Books to Read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{80050CA0-8D3E-48BA-BD84-E8E96811E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{785AFE10-494F-4E10-906B-39FFCA1E429C}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{80050CA0-8D3E-48BA-BD84-E8E96811E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C65DBD1-0AAD-4AE7-BC49-4DC30DDD2789}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB081F56-E215-4A57-8E05-68661072F278}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>ISBN</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>111-11-11111-11-1</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,6 +643,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>

</xml_diff>